<commit_message>
Use job arrival frequency instead of interarrival time in diagramm
Shows linear relationship of simulation time and load better.
</commit_message>
<xml_diff>
--- a/analysis/scalability_tests.xlsx
+++ b/analysis/scalability_tests.xlsx
@@ -66,7 +66,7 @@
     <t>Scalability regarding Load</t>
   </si>
   <si>
-    <t>Job Frequenz</t>
+    <t>Job Frequency</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1763,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Job Frequenz</c:v>
+                  <c:v>Job Frequency</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1978,8 +1978,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Interarrival Time in s</a:t>
+                  <a:t>Job</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> Arrival Frequency</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4853,8 +4858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="D24" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>